<commit_message>
add steering axle, refactor linear interpolation
</commit_message>
<xml_diff>
--- a/Data/brz.xlsx
+++ b/Data/brz.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tanut/Code/RoadBuilder/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C57344C-CD33-6046-A80C-21A4AAC646AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E3F798-BCED-7E49-B885-58F39EFD03B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="740" windowWidth="19380" windowHeight="16200" xr2:uid="{5059AB7A-6172-164E-8BAA-6883E59E2000}"/>
+    <workbookView xWindow="1480" yWindow="2520" windowWidth="23480" windowHeight="14780" xr2:uid="{5059AB7A-6172-164E-8BAA-6883E59E2000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">rpm (x) </t>
   </si>
@@ -49,11 +49,26 @@
   <si>
     <t>power kw (y2)</t>
   </si>
+  <si>
+    <t xml:space="preserve">slip angle (x) </t>
+  </si>
+  <si>
+    <t>lateral force (N)</t>
+  </si>
+  <si>
+    <t>normalized lateral force (N)</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -83,8 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -117,6 +133,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BRZ torque profile</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -565,7 +606,460 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>tyre slip angle</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>normalized lateral force (N)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$19:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$19:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82456140350877194</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92982456140350866</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98245614035087714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94736842105263164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.91228070175438591</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.89473684210526305</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8771929824561403</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.84210526315789469</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.82456140350877194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.82456140350877194</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0FAC-1041-8DB6-F67AB106C46B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1933895824"/>
+        <c:axId val="1945988880"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1933895824"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1945988880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1945988880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-TH"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1933895824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-TH"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-TH"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1108,20 +1602,523 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1141,6 +2138,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFA0A800-3994-96C0-C409-CE04904F5608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1446,14 +2479,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24625F7-ECDF-8340-90B8-1A77EA0604A8}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1550,6 +2584,170 @@
         <v>300</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <f>B19/$B$32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>4.7</v>
+      </c>
+      <c r="C20" s="1">
+        <f t="shared" ref="C20:C30" si="0">B20/$B$32</f>
+        <v>0.82456140350877194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>5.3</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.92982456140350866</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22">
+        <v>5.7</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>15</v>
+      </c>
+      <c r="B23">
+        <v>5.6</v>
+      </c>
+      <c r="C23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.98245614035087714</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>5.4</v>
+      </c>
+      <c r="C24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.94736842105263164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>5.2</v>
+      </c>
+      <c r="C25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.91228070175438591</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>30</v>
+      </c>
+      <c r="B26">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.89473684210526305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8771929824561403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>40</v>
+      </c>
+      <c r="B28">
+        <v>4.8</v>
+      </c>
+      <c r="C28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.84210526315789469</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>45</v>
+      </c>
+      <c r="B29">
+        <v>4.7</v>
+      </c>
+      <c r="C29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82456140350877194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>50</v>
+      </c>
+      <c r="B30">
+        <v>4.7</v>
+      </c>
+      <c r="C30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.82456140350877194</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32">
+        <f>MAX(B19:B30)</f>
+        <v>5.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>